<commit_message>
reservations text showing, testing needed
</commit_message>
<xml_diff>
--- a/applicationForm/dataPreparation/countryAPI/API articles with ratification dates and reservations.xlsx
+++ b/applicationForm/dataPreparation/countryAPI/API articles with ratification dates and reservations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\robolawyer\applicationForm\dataPreparation\countryAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B4CE64-B129-4A0D-B4C8-234030026D11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7E6BB7-F4A5-479F-AA44-B616288BCA88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="869" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="869" firstSheet="32" activeTab="47" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="with br CSV for API - New list " sheetId="1" r:id="rId1"/>
@@ -681,14 +681,6 @@
     <t>Azerbaijan made the following declaration upon the ratification of the European Convention on Human Rights: &lt;br/&gt; The Republic of Azerbaijan declares that it is unable to guarantee the application of the provisions of the Convention in the territories occupied by the Republic of Armenia until these territories are liberated from that occupation.</t>
   </si>
   <si>
-    <t>Derogations &lt;br/&gt; Azerbaijan temporarily derogated from its obligations under the provisions of Article 8 due to the entrance into force of the martial law in the Republic of Azerbaijan. The starting date of the derogation period is 28/09/2020. (For updated information, please check here [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=AZE ] 
-&lt;br/&gt; &lt;br/&gt; Declarations &lt;br/&gt; Azerbaijan made the following declaration upon the ratification of the European Convention on Human Rights: &lt;br/&gt; The Republic of Azerbaijan declares that it is unable to guarantee the application of the provisions of the Convention in the territories occupied by the Republic of Armenia until these territories are liberated from that occupation.</t>
-  </si>
-  <si>
-    <t>Derogations &lt;br/&gt; Azerbaijan temporarily derogated from its obligations under the provisions of Article 5 due to the entrance into force of the martial law in the Republic of Azerbaijan. The starting date of the derogation period is 28/09/2020. (For updated information, please check here [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=AZE ] 
-&lt;br/&gt; &lt;br/&gt; Declarations &lt;br/&gt; Azerbaijan made the following declaration upon the ratification of the European Convention on Human Rights: &lt;br/&gt; The Republic of Azerbaijan declares that it is unable to guarantee the application of the provisions of the Convention in the territories occupied by the Republic of Armenia until these territories are liberated from that occupation.</t>
-  </si>
-  <si>
     <t>Albania temporarily derogated from certain obligations under the provisions of Article 8 between 24/03/2020 - 24/06/2020.</t>
   </si>
   <si>
@@ -704,46 +696,7 @@
     <t>Albania temporarily derogated from certain obligations under the provisions of Article 2 of Protocol 4 between 24.03.2020 - 24.06.2020.</t>
   </si>
   <si>
-    <t>Armenia temporarily derogated from certain of its obligations under the provisions of Article 8 due to the entrance into force of the martial law in the Republic of Armenia. The starting date of the derogation period is 29/09/2020. (For updated information, please check here [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=ARM).</t>
-  </si>
-  <si>
-    <t>Armenia temporarily derogated from certain of its obligations under the provisions of Article 10 due to the entrance into force of the martial law in the Republic of Armenia. The starting date of the derogation period is 29/09/2020. (For updated information, please check here [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=ARM).</t>
-  </si>
-  <si>
-    <t>Armenia temporarily derogated from certain of its obligations under the provisions of Article 11 due to the entrance into force of the martial law in the Republic of Armenia. The starting date of the derogation period is 29/09/2020. (For updated information, please check here [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=ARM).</t>
-  </si>
-  <si>
-    <t>Armenia temporarily derogated from certain of its obligations under the provisions of Article 1 of Protocol 1 due to the entrance into force of the martial law in the Republic of Armenia. The starting date of the derogation period is 29/09/2020. (For updated information, please check here [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=ARM).</t>
-  </si>
-  <si>
-    <t>Armenia temporarily derogatedfrom certain of its obligations under the provisions of Article 2 of Protocol 4 due to the entrance into force of the martial law in the Republic of Armenia. The starting date of the derogation period is 29/09/2020. (For updated information, please check here [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=ARM).</t>
-  </si>
-  <si>
-    <t>Derogations &lt;br/&gt;&lt;br/&gt; Azerbaijan temporarily derogated from its obligations under the provisions of Article 2 of Protocol 4 due to the entrance into force of the martial law in the Republic of Azerbaijan. The starting date of the derogation period is 28/09/2020. (For updated information, please check here [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=AZE ] 
-&lt;br/&gt;&lt;br/&gt; &lt;br/&gt; Declarations &lt;br/&gt; &lt;br/&gt;Azerbaijan made the following declaration upon the ratification of the European Convention on Human Rights: &lt;br/&gt; The Republic of Azerbaijan declares that it is unable to guarantee the application of the provisions of the Convention in the territories occupied by the Republic of Armenia until these territories are liberated from that occupation.</t>
-  </si>
-  <si>
-    <t>Derogations &lt;br/&gt; &lt;br/&gt; Azerbaijan temporarily derogated from its obligations under the provisions of Article 11 due to the entrance into force of the martial law in the Republic of Azerbaijan. The starting date of the derogation period is 28/09/2020. (For updated information, please check here [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=AZE ] 
-&lt;br/&gt; &lt;br/&gt; &lt;br/&gt; Declarations &lt;br/&gt;  &lt;br/&gt; Azerbaijan made the following declaration upon the ratification of the European Convention on Human Rights: &lt;br/&gt; The Republic of Azerbaijan declares that it is unable to guarantee the application of the provisions of the Convention in the territories occupied by the Republic of Armenia until these territories are liberated from that occupation.</t>
-  </si>
-  <si>
-    <t>Derogations &lt;br/&gt; &lt;br/&gt; Azerbaijan temporarily derogated from its obligations under the provisions of Article 10 due to the entrance into force of the martial law in the Republic of Azerbaijan. The starting date of the derogation period is 28/09/2020. (For updated information, please check here [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=AZE ] 
-&lt;br/&gt;&lt;br/&gt;  &lt;br/&gt; Declarations &lt;br/&gt;&lt;br/&gt;  Azerbaijan made the following declaration upon the ratification of the European Convention on Human Rights: &lt;br/&gt; The Republic of Azerbaijan declares that it is unable to guarantee the application of the provisions of the Convention in the territories occupied by the Republic of Armenia until these territories are liberated from that occupation.</t>
-  </si>
-  <si>
-    <t>Derogations &lt;br/&gt;  &lt;br/&gt; Azerbaijan temporarily derogated from its obligations under the provisions of Article 5 due to the entrance into force of the martial law in the Republic of Azerbaijan. The starting date of the derogation period is 28/09/2020. (For updated information, please check here [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=AZE ] 
-&lt;br/&gt;&lt;br/&gt;  &lt;br/&gt; Declarations&lt;br/&gt;  &lt;br/&gt; Azerbaijan made the following declaration upon the ratification of the European Convention on Human Rights: &lt;br/&gt; The Republic of Azerbaijan declares that it is unable to guarantee the application of the provisions of the Convention in the territories occupied by the Republic of Armenia until these territories are liberated from that occupation.</t>
-  </si>
-  <si>
-    <t>Derogations &lt;br/&gt;&lt;br/&gt; Azerbaijan temporarily derogated from certain obligations under the provisions of Article 1 of Protocol 1 due to the entrance into force of the martial law in the Republic of Azerbaijan. The starting date of the derogation period is 28/09/2020. (For updated information, please check here [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=AZE ] 
-&lt;br/&gt;&lt;br/&gt; &lt;br/&gt; Declarations &lt;br/&gt;&lt;br/&gt; Azerbaijan made the following declaration upon the ratification of the European Convention on Human Rights: &lt;br/&gt; The Republic of Azerbaijan declares that it is unable to guarantee the application of the provisions of the Convention in the territories occupied by the Republic of Armenia until these territories are liberated from that occupation.</t>
-  </si>
-  <si>
     <t>Belgium made the following declaration concerning the provisions of Article 1 of Protocol 7: &lt;br/&gt; Belgium understands the words "resident" and "lawfully" mentioned in Article 1 of this Protocol in the sense that is given to them in paragraph 9 of its Explanatory Report. &lt;br/&gt; The declaration was made on 11/05/2005.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Derogations &lt;br/&gt;&lt;br/&gt; Azerbaijan temporarily derogated from its obligations under the provisions of Article 2 of Protocol 1 due to the entrance into force of the martial law in the Republic of Azerbaijan. The starting date of the derogation period is 28/09/2020. (For updated information, please check here [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=AZE ] 
-&lt;br/&gt;&lt;br/&gt; &lt;br/&gt; Declarations &lt;br/&gt;&lt;br/&gt; Azerbaijan made the following declarations upon the ratification of the European Convention on Human Rights: &lt;br/&gt;1. The Republic of Azerbaijan declares that it is unable to guarantee the application of the provisions of the Convention in the territories occupied by the Republic of Armenia until these territories are liberated from that occupation. &lt;br/&gt;&lt;br/&gt; 2. The Republic of Azerbaijan declares that it interprets the second sentence of Article 2 of the Protocol in the sense that this provision does not impose on the State any obligation to finance religious education. </t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria made the following reservation to the provisions of Article 1 of Protocol 1: &lt;br/&gt; &lt;br/&gt; The terms of the second provision of Article 1 of the Protocol shall not affect the scope or content of Article 22, paragraph 1, of the Constitution of the Republic of Bulgaria, which states that : "No foreign physical person or foreign legal entity shall acquire ownership over land, except through legal inheritance. Ownership thus acquired shall be duly transferred." </t>
@@ -796,27 +749,6 @@
     <t>Territorial application &lt;br/&gt;&lt;br/&gt;Denmark made a territorial reservation upon the ratification of Protocol 13 stating that the said Protocol shall not apply to the Faroe Islands and Greenland. &lt;br/&gt; The territorial reservation concerning the Faroe Islands was withdrawn on 01/11/2003 and the territorial reservation concerning Greenland was withdrawn on 01/05/2004.</t>
   </si>
   <si>
-    <t>Estonia temporarily derogated from certain of its obligations under the provisions of Article 5 during the emergency situation pursuant to the COVID-19 pandemic. Period covered by the derogation: 20/03/2020 - 18/05/2020. You can find more information about the derogation here. [Hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=EST ]</t>
-  </si>
-  <si>
-    <t>Estonia temporarily derogated from certain of its obligations under the provisions of Article 8 during the emergency situation pursuant to the COVID-19 pandemic. Period covered by the derogation: 20/03/2020 - 18/05/2020. You can find more information about the derogation here. [Hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=EST ]</t>
-  </si>
-  <si>
-    <t>Estonia temporarily derogated from certain of its obligations under the provisions of Article 11 during the emergency situation pursuant to the COVID-19 pandemic. Period covered by the derogation: 20/03/2020 - 18/05/2020. You can find more information about the derogation here. [Hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=EST ]</t>
-  </si>
-  <si>
-    <t>Estonia temporarily derogated from certain of its obligations under the provisions of Article 2 of Protocol 4 during the emergency situation pursuant to the COVID-19 pandemic. Period covered by the derogation: 20/03/2020 - 18/05/2020. You can find more information about the derogation here. [Hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/046/declarations?p_auth=5IOZ28jl&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=EST ]</t>
-  </si>
-  <si>
-    <t>Estonia temporarily derogated from certain of its obligations under the provisions of Article 2 of Protocol 1 during the emergency situation pursuant to the COVID-19 pandemic. Period covered by the derogation: 20/03/2020 - 18/05/2020. You can find more information about the derogation here. [Hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/009/declarations?p_auth=5IOZ28jl&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=EST ]</t>
-  </si>
-  <si>
-    <t>Reservations &lt;br/&gt; &lt;br/&gt; Estonia made the following reservation  to the provisions of Article 1 of Protocol 1: &lt;br/&gt;&lt;br/&gt;  In accordance with Article 64 of the Convention, the Republic of Estonia declares that the provisions of Article 1 of the First Protocol shall not apply to the laws on property reform which regulate the restoration or compensation of property nationalised, confiscated, requisitioned, collectivised or otherwise unlawfully expropriated during the period of Soviet annexation; the restructuring of collectivised agriculture and privatisation of state owned property. The reservation concerns the Principles of the Property Reform Act (published in Riigi Teataja [State Gazette] 1991, 21, 257; RT I 1994, 38, 617; 40, 653; 51, 859; 94, 1609), the Land Reform Act (RT 1991, 34, 426; RT I 1995,, 10, 113), the Agricultural Reform Act (RT 1992, 10, 143; 36, 474; RT I 1994, 52, 880), the Privatisation Act (RT I 1993, 45, 639; 1994, 50, 846; 79, 1329; 83, 1448; 1995, 22, 327; 54, 881; 57, 979), the Dwelling Rooms Privatisation Act (RT I 1993, 23, 411; 1995, 44, 671; 57, 979; 1996, 2, 28), the Act on Evaluation and Compensation of Unlawfully Expropriated Property (RT I 1993, 30, 509; 1994, 8, 106; 51, 859; 54, 905; 1995, 29, 357), the Act on Evaluation of Collectivised Property (RT I 1993, 7, 104) and their wording being in force at the moment of the Ratification Act entered into force. &lt;br/&gt;&lt;br/&gt;&lt;br/&gt; Derogations &lt;br/&gt; Estonia temporarily derogated from certain of its obligations under the provisions of Article 1 of Protocol 1 during the emergency situation pursuant to the COVID-19 pandemic. Period covered by the derogation: 20/03/2020 - 18/05/2020. You can find more information about the derogation here. [Hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/009/declarations?p_auth=5IOZ28jl&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=EST ]</t>
-  </si>
-  <si>
-    <t>Reservations &lt;br/&gt; &lt;br/&gt; Estonia made the following reservation to the provisions of Article 6: &lt;br/&gt; The Republic of Estonia, in accordance with Article 64 of the Convention [Article 57 since the entry into force of the Protocol No 11], declares that while pending the adoption of amendments to the Code on Civil Procedure within one year from entry into force of the Ratification Act, she cannot ensure the right to a public hearing at the appellate court level (Ringkonnakohtus) as provided in Article 6 of the Convention, in so far as cases foreseen by Articles 292 and 298 of the Code on Civil Procedure (published in the Riigi Teataja [State Gazette] I 1993, 31/32, 538; 1994, 1, 5; 1995, 29, 358; 1996, 3, 57) may be decided through written procedure.    &lt;br/&gt; &lt;br/&gt;  &lt;br/&gt;Derogations &lt;br/&gt; Estonia temporarily derogated from certain of its obligations under the provisions of Article 6 during the emergency situation pursuant to the COVID-19 pandemic. Period covered by the derogation: 20/03/2020 - 18/05/2020. You can find more information about the derogation here. [Hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=EST ]</t>
-  </si>
-  <si>
     <t>Finland made the following reservation to the provisions of Article 6: &lt;br/&gt;For the time being, Finland cannot guarantee a right to an oral hearing insofar as the current Finnish laws do not provide such a right. This applies to:  &lt;br/&gt;
 1. proceedings before the Supreme Court in accordance with Chapter 30, Section 20, of the Code of Judicial Procedure and proceedings before the Courts of Appeal as regards the consideration of petition, civil and criminal cases to which Chapter 26 (661/1978), Sections 7 and 8, of the Code of Judicial Procedure are applied if the decision of a District Court has been made before 1 May 1998, when the amendments made to the provisions concerning proceedings before Courts of Appeal entered into force;
 and the consideration of criminal cases before the Supreme Court and the Courts of Appeal if the case has been pending before a District Court at the time of entry into force of the Criminal Proceedings Act on 1 October 1997 and to which existing provisions have been applied by the District Court;  &lt;br/&gt;
@@ -860,33 +792,7 @@
     <t>France made the following declaration concerning the territorial application of Protocol 7: &lt;br/&gt; The Protocol shall apply to the whole territory of the Republic, due regard being had where the overseas territories and the territorial collectivity of Mayotte are concerned, to the local requirements referred to in Article 63 [Article 56 since the entry into force of Protocol No. 11] of the European Convention on Human Rights and Fundamental Freedoms.</t>
   </si>
   <si>
-    <t>Georgia temporarily derogated from certain of its obligations under the provisions of Article 8 due to the COVID-19 pandemic. The derogation period started on 23/03/2020. (For updated information on the ongoing derogation, please check here).  [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=GEO].</t>
-  </si>
-  <si>
-    <t>Georgia temporarily derogated from certain of its obligations under the provisions of Article 5 due to the COVID-19 pandemic. The derogation period started on 23/03/2020. (For updated information on the ongoing derogation, please check here).  [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=GEO].</t>
-  </si>
-  <si>
-    <t>Georgia temporarily derogated from certain of its obligations under the provisions of Article 6 due to the COVID-19 pandemic. The derogation period started on 23/03/2020. (For updated information on the ongoing derogation, please check here).  [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=GEO].</t>
-  </si>
-  <si>
     <t>Georgia made the following declaration upon ratidication of Protocol 1:&lt;br/&gt; Due to the existing situation in Abkhazia and Tskhinvali region, Georgian authorities are unable to undertake commitments concerning the respect and protection of the provisions of the Convention and its Additional Protocols on these territories. Georgia therefore declines its responsibility for violations of the provisions of the Protocol by the organs of self-proclaimed illegal forces on the territories of Abkhazia and Tskhinvali region until the possibility of realization of the full jurisdiction of Georgia is restored over these territories</t>
-  </si>
-  <si>
-    <t>Georgia temporarily derogated from certain of its obligations under the provisions of Article 2 of Protocol 4 due to the COVID-19 pandemic. The derogation period started on 23/03/2020. (For updated information on the ongoing derogation, please check here).  [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/046/declarations?p_auth=5IOZ28jl&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=GEO ]</t>
-  </si>
-  <si>
-    <t>Reservations &lt;br/&gt;&lt;br/&gt; Georgia made the following reservation to the provisions of Article 1 of Protocol 1: &lt;br/&gt;1. Article 1 of the Protocol shall not apply to persons who have or will obtain status of “internally displaced persons” in accordance with “the Law of Georgia on Internally Displaced Persons” until the elimination of circumstances motivating the granting of this status (until the restoration of the territorial integrity of Georgia). In accordance with the aforementioned law, Georgia assumes responsibility to ensure the exercise of rights over property that exist on the place of permanent residence of internally displaced persons after the reasons mentioned in Article 1, paragraph 1, of this law have been eliminated.
-&lt;br/&gt; 
-2. Article 1 of the Protocol shall be applied to the operational sphere of “the Law of Georgia on the Ownership of Agricultural Land” in accordance with the requirements of Articles 4, 8, 15 and 19 of this Law.
-&lt;br/&gt; 
-3. Article 1 of the Protocol shall be applied within the limits of Articles 2 and 3 of the Law of Georgia on Transference into Private Property of the Non-Agricultural Lands Being in Possession of Natural Persons and Legal Persons of Private Law”.
-&lt;br/&gt; 
-4. Article 1 of the Protocol shall be applied within the limits of the “Law of Georgia on Privatisation of the State Property”. &lt;br/&gt; 
-5. With regard to the compensation of pecuniary assets placed on accounts of the former Georgian public-commercial banks, Article 1 of the Protocol shall be applied within the limits of the normative act adopted in pursuance of the Decree No. 258 of the President of Georgia of 2 July 2001.  &lt;br/&gt; &lt;br/&gt; Derogations &lt;br/&gt; Georgia has derogated from Article 1 of Protocol 1 during 03/03/2006 - 16/03/2006 and during the COVID-19 pandemic state of emergency which was instituted on 15/07/2020. &lt;br/&gt; &lt;br/&gt; Declarations &lt;br/&gt;Georgia made the following declaration upon ratidication of Protocol 1:&lt;br/&gt; Due to the existing situation in Abkhazia and Tskhinvali region, Georgian authorities are unable to undertake commitments concerning the respect and protection of the provisions of the Convention and its Additional Protocols on these territories. Georgia therefore declines its responsibility for violations of the provisions of the Protocol by the organs of self-proclaimed illegal forces on the territories of Abkhazia and Tskhinvali region until the possibility of realization of the full jurisdiction of Georgia is restored over these territories. The declaration is active since 07/06/2002.
- &lt;br/&gt; &gt;br/&gt; &lt;br/&gt; Derogations &lt;br/&gt; &gt;br/&gt; Georgia temporarily derogated from certain of its obligations under the provisions of Article 1 of Protocol 1 due to the COVID-19 pandemic. The derogation period started on 23/03/2020. (For updated information on the ongoing derogation, please check here).  [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/009/declarations?p_auth=5IOZ28jl&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=GEO  ].</t>
-  </si>
-  <si>
-    <t>Reservations &lt;br/&gt;&lt;br/&gt; Georgia made the following reservation to the provisions of Article 2 of Protocol 1: &lt;br/&gt; Georgia declares that it interprets Article 2 of the Protocol as not imposing on the State additional financial commitments relating to special educational establishments (with a specific philosophical or religious orientation) other than those provided by the legislation of Georgia.  &lt;br/&gt; &lt;br/&gt;&lt;br/&gt; Derogations &lt;br/&gt; Georgia temporarily derogated from certain of its obligations under the provisions of Article 2 of Protocol 1 during the COVID-19 pandemic state of emergency which was instituted on 15/07/2020. (For updated information on the ongoing derogation, please check here).  [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/009/declarations?p_auth=5IOZ28jl&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=GEO  ]. &lt;br/&gt; &lt;br/&gt;&lt;br/&gt; Declarations &lt;br/&gt; Georgia made the following declaration upon ratidication of Protocol 1: &lt;br/&gt; Due to the existing situation in Abkhazia and Tskhinvali region, Georgian authorities are unable to undertake commitments concerning the respect and protection of the provisions of the Convention and its Additional Protocols on these territories. Georgia therefore declines its responsibility for violations of the provisions of the Protocol by the organs of self-proclaimed illegal forces on the territories of Abkhazia and Tskhinvali region until the possibility of realization of the full jurisdiction of Georgia is restored over these territories.</t>
   </si>
   <si>
     <t>Georgia made the following declaration concerning the provisions of Protocol 12:&lt;br/&gt; Georgia declines its responsibility for the violations of the provisions of the Protocol on the territories of Abkhazia and Tskhinvali region until the full jurisdiction of Georgia is restored over these territories.</t>
@@ -1214,27 +1120,6 @@
 &lt;br/&gt; Article 3 of the said Law No. 6366 reads: &lt;br/&gt; Article 2 of the Protocol shall not affect the provisions of Law No. 430 of 3 March 1924 relating to the unification of education.</t>
   </si>
   <si>
-    <t>Ukraine declared public emergency pursuant to the conflict in north-eastern Ukraine and derogated from certain of its obligations under the provisions of Article 13. Period covered: 09/06/2015 – ongoing. For further details regarding the state of emergency, please visit this page. [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=U</t>
-  </si>
-  <si>
-    <t>Reservations &lt;br/&gt;&lt;br/&gt;
-Ukraine made the following reservation to the provisions of Article 8: &lt;br/&gt;  The provisions of Article 8 of the Convention for the Protection of Human Rights and Fundamental Freedoms of 1950 shall apply in the part that does not contradict paragraph 13 of Chapter XV "Transitional Provisions" of the Constitution of Ukraine and Articles 177 and 190 of the Criminal Procedure Code of Ukraine concerning warrants for arrest and search warrants issued by the public prosecutor. Period covered: 11/09/1997 - 28/06/2001.
-&lt;br/&gt;&lt;br/&gt; &lt;br/&gt;Derogations. &lt;br/&gt;&lt;br/&gt; Ukraine declared public emergency pursuant to the conflict in north-eastern Ukraine and derogated from certain of its obligations under the provisions of Article 8. Period covered: 09/06/2015 – ongoing. For further details regarding the state of emergency, please visit this page. [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=U</t>
-  </si>
-  <si>
-    <t>Reservations &lt;br/&gt; &lt;br/&gt; Ukraine made the following reservations to the provisions of Article 5: &lt;br/&gt; The provisions of Article 5, paragraph 3, of the Convention for the Protection of Human Rights and Fundamental Freedoms of 1950 shall apply in the part that does not contradict paragraphs 50, 51, 52 and 53 of the Interim Disciplinary Statute of the Armed Forces of Ukraine approved by the Decree No 431 of the President of Ukraine dated 7 October 1993, concerning the imposition of arrest as a disciplinary sanction. &lt;br/&gt; &lt;br/&gt; (Period covered: 11/09/1997 - 29/06/2001) The provisions of Article 5, paragraph 1, of the Convention for the Protection of Human Rights and Fundamental Freedoms of 1950 shall apply in the part that does not contradict paragraph 13 of Chapter XV of the Transitional Provisions of the Constitution of Ukraine and Articles 106 and 157 of the Criminal Procedure Code of Ukraine concerning the detention of a person and the arrest warrant issued by the public prosecutor.  
-&lt;br/&gt; &lt;br/&gt; &lt;br/&gt;Derogations. &lt;br/&gt; &lt;br/&gt; Ukraine declared public emergency pursuant to the conflict in north-eastern Ukraine and derogated from certain of its obligations under the provisions of Article 5. Period covered: 09/06/2015 – ongoing. For further details regarding the state of emergency, please visit this page. [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=U</t>
-  </si>
-  <si>
-    <t>Reservations &lt;br/&gt; &lt;br/&gt; 
-Ukraine made the following reservations to the provisions of Article 6: &lt;br/&gt;
-Ukraine fully recognises on its territory the validity of Article 6, paragraph 3.d, of the Convention for the Protection of Human Rights and Fundamental Freedoms of 1950 in regard to the defendant's right to obtain the attendance and examination of witnesses (Articles 263 and 303 of the Criminal Procedure Code of Ukraine) and as regards the rights of the suspect and persons charged in pre-trial proceedings to submit petitions for the attendance and examination of witnesses and the confrontation with them in accordance with Articles 43, 431 and 142 of the above-mentioned Code.
-&lt;br/&gt; &lt;br/&gt; &lt;br/&gt;Derogations. &lt;br/&gt; &lt;br/&gt;  Ukraine declared public emergency pursuant to the conflict in north-eastern Ukraine and derogated from certain of its obligations under the provisions of  Article 6. Period covered: 09/06/2015 – ongoing. For further details regarding the state of emergency, please visit this page. [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=U</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ukraine declared public emergency pursuant to the conflict in north-eastern Ukraine and derogated from certain of its obligations under the provisions of Article 2 of Protocol 4. . Period covered: 09/06/2015 – ongoing. Please follow this link for further details: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=i2TjEjny&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=U&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10 </t>
-  </si>
-  <si>
     <t>Ukraine made the following declaration concerning the provisions of Protocol 6: &lt;br/&gt; On 29 December 1999, the Constitutional Court of Ukraine ruled that the provisions of the Criminal Code of Ukraine which provided for death penalty were unconstitutional. According to the Law of Ukraine of 22 February 2000 "On the Introduction of Amendments to the Criminal, Criminal Procedure and Correctional Labour Codes of Ukraine", the Criminal Code of Ukraine has been brought into conformity with the above-mentioned ruling of the Constitutional Court of Ukraine. The death penalty was replaced by life imprisonment (Article 25 of the Criminal Code of Ukraine). The Law of Ukraine "On the ratification of Protocol No. 6 to the Convention for the Protection of Human Rights and Fundamental Freedoms concerning the abolition of the Death Penalty, of 1983" envisages retaining of application of the death penalty for offences committed in time of war by means of introduction of appropriate amendments to the legislation in force.
 &lt;br/&gt;
 Pursuant to Article 2 of the Protocol No. 6 to the Convention for the Protection of Human Rights and Fundamental Freedoms, Ukraine will notify the Secretary General of the Council of Europe in case of introduction of these amendments.</t>
@@ -1243,12 +1128,6 @@
     <t xml:space="preserve">Ukraine made the following declaration concerning the provisions of Protocol 6: &lt;br/&gt; On 29 December 1999, the Constitutional Court of Ukraine ruled that the provisions of the Criminal Code of Ukraine which provided for death penalty were unconstitutional. According to the Law of Ukraine of 22 February 2000 "On the Introduction of Amendments to the Criminal, Criminal Procedure and Correctional Labour Codes of Ukraine", the Criminal Code of Ukraine has been brought into conformity with the above-mentioned ruling of the Constitutional Court of Ukraine. The death penalty was replaced by life imprisonment (Article 25 of the Criminal Code of Ukraine). The Law of Ukraine "On the ratification of Protocol No. 6 to the Convention for the Protection of Human Rights and Fundamental Freedoms concerning the abolition of the Death Penalty, of 1983" envisages retaining of application of the death penalty for offences committed in time of war by means of introduction of appropriate amendments to the legislation in force.
 &lt;br/&gt;
 Pursuant to Article 2 of the Protocol No. 6 to the Convention for the Protection of Human Rights and Fundamental Freedoms, Ukraine will notify the Secretary General of the Council of Europe in case of introduction of these amendments. </t>
-  </si>
-  <si>
-    <t>Ukraine declared public emergency pursuant to the conflict in north-eastern Ukraine and triggered Article 15 from 09/06/2015 onwards. For further details regarding the state of emergency, please visit this page. [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=U</t>
-  </si>
-  <si>
-    <t>Turkey declared state of emergency and triggered Article 15, thereby derogating from certain of its obligations under the European Convention on Human Rights, during the following periods: 28/02/1961 - 19/12/1961, 28/05/1963 - 29/07/1964, 19/06/1970 - 19/09/1970, 04/05/1971 - 26/09/1973, 24/07/1974 - 05/08/1975, 28/12/1978 - 19/07/1987, 06/08/1990 - 29/01/2002, 21/07/2016 - 19/07/2018. For more information please check here. [Hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=TUR</t>
   </si>
   <si>
     <t>Serbia triggered Article 15 during the COVID-19 pandemic and derogated from certain of its obligations under the European Convention on Human Rights. Period covered: 06/04/2020 - 06/05/2020</t>
@@ -1269,19 +1148,10 @@
     <t>Latvia has triggered Article 15 during the COVID-19 pandemic. Period covered: 16/03/2020 - 10/06/2020.</t>
   </si>
   <si>
-    <t>Georgia triggered Article 15 during the following periods: 03/03/2006 - 16/03/2006 due to the H5N1 virus, 09/11/2007 - 16/11/2007 due to a coup d'Etat, and since 23/03/2020 onwards due to the COVID-19 pandemic.  For updated information on the ongoing derogation, please check here.  [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=GEO].</t>
-  </si>
-  <si>
-    <t>Georgia temporarily derogated from certain of its obligations under the provisions of Article 8 due to the COVID-19 pandemic. The derogation period started on 23/03/2020. For updated information on the ongoing derogation, please check here.  [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=GEO].</t>
-  </si>
-  <si>
     <t>Reservations &lt;br/&gt; &lt;br/&gt; France made the following reservation to the provisions of Article 15: &lt;br/&gt; &lt;br/&gt; The Government of the Republic, in accordance with Article 64 of the Convention [Article 57 since the entry into force of the Protocol No 11], makes a reservation in respect of paragraph 1 of Article 15, to the effect, firstly, that the circumstances specified in Article 16 of the Constitution regarding the implementation of that Article, in Section 1 of the Act of 3 April 1878 and in the Act of 9 August 1849 regarding proclamation of a state of siege, and in Section 1 of Act No. 55-385 of 3 April 1955 regarding proclamation of a state of emergency, and in which it is permissible to apply the provisions of those texts, must be understood as complying with the purpose of Article 15 of the Convention and that, secondly, for the interpretation and application of Article 16 of the Constitution of the Republic, the terms to the extent strictly required by the exigencies of the situation shall not restrict the power of the President of the Republic to take the measures required by the circumstances. &lt;br/&gt;&lt;br/&gt; &lt;br/&gt;Derogations &lt;br/&gt; &lt;br/&gt; France declared state of emergency and triggered Article 15 for the following periods of time: 24/11/2015 - 01/11/2017 and 08/02/1985 - 30/06/1985. &lt;br/&gt; &gt;br/&gt; &lt;br/&gt; Territorial application &lt;br/&gt; France made the following declaration concerning the territorial application of the European Convention on Human Rights: &lt;br/&gt; The Government of the Republic further declares that the Convention shall apply to the whole territory of the Republic, having due regard, where the overseas territories are concerned, to local requirements, as mentioned in Article 63 [Article 56 since the entry into force of the Protocol No 11].</t>
   </si>
   <si>
     <t>Estonia triggered Article 15 during the COVID-19 pandemic and derogated from certain obligations under Articles 8, 6, 5, 15 and 11 of the European Convention on Human Rights, Articles 1 and 2 of Protocol1 and Article 2 of Protocol No.4. Period covered: 20/03/2020 - 18/05/2020.</t>
-  </si>
-  <si>
-    <t>Armenia triggered Article 15 during the following periods of time: 04/03/2008 - 21/03/2008, 19/03/2020 - 11/09/2020, and from 29/09/2020 onwards. (For updated information, please check here [hyperlink: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=ARM).</t>
   </si>
   <si>
     <t>Albania triggered Article 15 during the COVID-19 pandemic and derogated from certain obligations of Republic of Albania under Articles 8 and 11 of the Convention for the Protection of Human Rights and Fundamental Freedom, Articles 1 and 2 of Protocol to the Convention for the Protection of Human Rights and Fundamental Freedom and Article 2 of Protocol No.4 to the Convention for the Protection of Human Rights and Fundamental Freedom. Period covered: 24.03.2020 - 24.06.2020.</t>
@@ -1299,7 +1169,156 @@
 Territorial extension accepted on a permanent basis as from 22 November 2010: Anguilla, Bermuda, Montserrat, St Helena, Ascension and Tristan da Cunha &lt;br/&gt;</t>
   </si>
   <si>
-    <t>Derogations &lt;br/&gt; &lt;br/&gt; The United Kingdom triggered Article 15 during the following periods: [derogations before 01/09/1966, though existing, are not mentioned] 01/09/1966 - 30/11/1967, 25/09/1969 - 22/08/1984, 23/12/1988 - 05/05/2006, when certain provisions of the European Convention on Human Rights are derogated from. For further details, see: https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=i2TjEjny&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=UK&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10    Territorial application &lt;br/&gt; &lt;br/&gt;
+    <t>Armenia temporarily derogated from certain of its obligations under the provisions of Article 8 due to the entrance into force of the martial law in the Republic of Armenia. The starting date of the derogation period is 29/09/2020. (For updated information, please &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=ARM" target="_blank"&gt;check here&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Armenia temporarily derogated from certain of its obligations under the provisions of Article 10 due to the entrance into force of the martial law in the Republic of Armenia. The starting date of the derogation period is 29/09/2020. (For updated information, please &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=ARM" target="_blank"&gt;check here&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Armenia temporarily derogated from certain of its obligations under the provisions of Article 11 due to the entrance into force of the martial law in the Republic of Armenia. The starting date of the derogation period is 29/09/2020. (For updated information, please &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=ARM" target="_blank"&gt;check here&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Armenia triggered Article 15 during the following periods of time: 04/03/2008 - 21/03/2008, 19/03/2020 - 11/09/2020, and from 29/09/2020 onwards. (For updated information, please &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=ARM" target="_blank"&gt;check here&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Armenia temporarily derogated from certain of its obligations under the provisions of Article 1 of Protocol 1 due to the entrance into force of the martial law in the Republic of Armenia. The starting date of the derogation period is 29/09/2020. (For updated information, please &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=ARM" target="_blank"&gt;check here&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Armenia temporarily derogatedfrom certain of its obligations under the provisions of Article 2 of Protocol 4 due to the entrance into force of the martial law in the Republic of Armenia. The starting date of the derogation period is 29/09/2020. (For updated information, please &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=ARM" target="_blank"&gt; check here &lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Derogations &lt;br/&gt; Azerbaijan temporarily derogated from its obligations under the provisions of Article 5 due to the entrance into force of the martial law in the Republic of Azerbaijan. The starting date of the derogation period is 28/09/2020. (For updated information, please &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=AZE" target="_blank"&gt; check here&lt;/a&gt;. 
+&lt;br/&gt; &lt;br/&gt; Declarations &lt;br/&gt; Azerbaijan made the following declaration upon the ratification of the European Convention on Human Rights: &lt;br/&gt; The Republic of Azerbaijan declares that it is unable to guarantee the application of the provisions of the Convention in the territories occupied by the Republic of Armenia until these territories are liberated from that occupation.</t>
+  </si>
+  <si>
+    <t>Derogations &lt;br/&gt;  &lt;br/&gt; Azerbaijan temporarily derogated from its obligations under the provisions of Article 5 due to the entrance into force of the martial law in the Republic of Azerbaijan. The starting date of the derogation period is 28/09/2020. (For updated information, please &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=AZE" target="_blank"&gt;check here&lt;/a&gt; 
+&lt;br/&gt;&lt;br/&gt;  &lt;br/&gt; Declarations&lt;br/&gt;  &lt;br/&gt; Azerbaijan made the following declaration upon the ratification of the European Convention on Human Rights: &lt;br/&gt; The Republic of Azerbaijan declares that it is unable to guarantee the application of the provisions of the Convention in the territories occupied by the Republic of Armenia until these territories are liberated from that occupation.</t>
+  </si>
+  <si>
+    <t>Derogations &lt;br/&gt; Azerbaijan temporarily derogated from its obligations under the provisions of Article 8 due to the entrance into force of the martial law in the Republic of Azerbaijan. The starting date of the derogation period is 28/09/2020. (For updated information, please &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=AZE" target="_blank"&gt;check here&lt;/a&gt;. 
+&lt;br/&gt; &lt;br/&gt; Declarations &lt;br/&gt; Azerbaijan made the following declaration upon the ratification of the European Convention on Human Rights: &lt;br/&gt; The Republic of Azerbaijan declares that it is unable to guarantee the application of the provisions of the Convention in the territories occupied by the Republic of Armenia until these territories are liberated from that occupation.</t>
+  </si>
+  <si>
+    <t>Derogations &lt;br/&gt; &lt;br/&gt; Azerbaijan temporarily derogated from its obligations under the provisions of Article 10 due to the entrance into force of the martial law in the Republic of Azerbaijan. The starting date of the derogation period is 28/09/2020. (For updated information, please &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=AZE" target="_blank"&gt;check here&lt;/a&gt; 
+&lt;br/&gt;&lt;br/&gt;  &lt;br/&gt; Declarations &lt;br/&gt;&lt;br/&gt;  Azerbaijan made the following declaration upon the ratification of the European Convention on Human Rights: &lt;br/&gt; The Republic of Azerbaijan declares that it is unable to guarantee the application of the provisions of the Convention in the territories occupied by the Republic of Armenia until these territories are liberated from that occupation.</t>
+  </si>
+  <si>
+    <t>Derogations &lt;br/&gt; &lt;br/&gt; Azerbaijan temporarily derogated from its obligations under the provisions of Article 11 due to the entrance into force of the martial law in the Republic of Azerbaijan. The starting date of the derogation period is 28/09/2020. (For updated information, please &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=AZE" target="_blank"&gt; check here&lt;/a&gt;  
+&lt;br/&gt; &lt;br/&gt; &lt;br/&gt; Declarations &lt;br/&gt;  &lt;br/&gt; Azerbaijan made the following declaration upon the ratification of the European Convention on Human Rights: &lt;br/&gt; The Republic of Azerbaijan declares that it is unable to guarantee the application of the provisions of the Convention in the territories occupied by the Republic of Armenia until these territories are liberated from that occupation.</t>
+  </si>
+  <si>
+    <t>Derogations &lt;br/&gt;&lt;br/&gt; Azerbaijan temporarily derogated from certain obligations under the provisions of Article 1 of Protocol 1 due to the entrance into force of the martial law in the Republic of Azerbaijan. The starting date of the derogation period is 28/09/2020. (For updated information, please &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=AZE" target="_blank"&gt; check here&lt;/a&gt;
+&lt;br/&gt;&lt;br/&gt; &lt;br/&gt; Declarations &lt;br/&gt;&lt;br/&gt; Azerbaijan made the following declaration upon the ratification of the European Convention on Human Rights: &lt;br/&gt; The Republic of Azerbaijan declares that it is unable to guarantee the application of the provisions of the Convention in the territories occupied by the Republic of Armenia until these territories are liberated from that occupation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Derogations &lt;br/&gt;&lt;br/&gt; Azerbaijan temporarily derogated from its obligations under the provisions of Article 2 of Protocol 1 due to the entrance into force of the martial law in the Republic of Azerbaijan. The starting date of the derogation period is 28/09/2020. (For updated information, please &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=AZE" target="_blank"&gt;check here&lt;/a&gt;
+&lt;br/&gt;&lt;br/&gt; &lt;br/&gt; Declarations &lt;br/&gt;&lt;br/&gt; Azerbaijan made the following declarations upon the ratification of the European Convention on Human Rights: &lt;br/&gt;1. The Republic of Azerbaijan declares that it is unable to guarantee the application of the provisions of the Convention in the territories occupied by the Republic of Armenia until these territories are liberated from that occupation. &lt;br/&gt;&lt;br/&gt; 2. The Republic of Azerbaijan declares that it interprets the second sentence of Article 2 of the Protocol in the sense that this provision does not impose on the State any obligation to finance religious education. </t>
+  </si>
+  <si>
+    <t>Derogations &lt;br/&gt;&lt;br/&gt; Azerbaijan temporarily derogated from its obligations under the provisions of Article 2 of Protocol 4 due to the entrance into force of the martial law in the Republic of Azerbaijan. The starting date of the derogation period is 28/09/2020. (For updated information, please &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=AZE" target="_blank"&gt; check here&lt;/a&gt;  
+&lt;br/&gt;&lt;br/&gt; &lt;br/&gt; Declarations &lt;br/&gt; &lt;br/&gt;Azerbaijan made the following declaration upon the ratification of the European Convention on Human Rights: &lt;br/&gt; The Republic of Azerbaijan declares that it is unable to guarantee the application of the provisions of the Convention in the territories occupied by the Republic of Armenia until these territories are liberated from that occupation.</t>
+  </si>
+  <si>
+    <t>Estonia temporarily derogated from certain of its obligations under the provisions of Article 5 during the emergency situation pursuant to the COVID-19 pandemic. Period covered by the derogation: 20/03/2020 - 18/05/2020. You can find more information about the derogation &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=EST" target="_blank"&gt;here&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reservations &lt;br/&gt; &lt;br/&gt; Estonia made the following reservation to the provisions of Article 6: &lt;br/&gt; The Republic of Estonia, in accordance with Article 64 of the Convention [Article 57 since the entry into force of the Protocol No 11], declares that while pending the adoption of amendments to the Code on Civil Procedure within one year from entry into force of the Ratification Act, she cannot ensure the right to a public hearing at the appellate court level (Ringkonnakohtus) as provided in Article 6 of the Convention, in so far as cases foreseen by Articles 292 and 298 of the Code on Civil Procedure (published in the Riigi Teataja [State Gazette] I 1993, 31/32, 538; 1994, 1, 5; 1995, 29, 358; 1996, 3, 57) may be decided through written procedure.    &lt;br/&gt; &lt;br/&gt;  &lt;br/&gt;Derogations &lt;br/&gt; Estonia temporarily derogated from certain of its obligations under the provisions of Article 6 during the emergency situation pursuant to the COVID-19 pandemic. Period covered by the derogation: 20/03/2020 - 18/05/2020. You can find more information about the derogation &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=EST" target="_blank"&gt;here&lt;/a&gt;. </t>
+  </si>
+  <si>
+    <t>Estonia temporarily derogated from certain of its obligations under the provisions of Article 8 during the emergency situation pursuant to the COVID-19 pandemic. Period covered by the derogation: 20/03/2020 - 18/05/2020. You can find more information about the derogation &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=EST" target="_blank"&gt;here&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Estonia temporarily derogated from certain of its obligations under the provisions of Article 11 during the emergency situation pursuant to the COVID-19 pandemic. Period covered by the derogation: 20/03/2020 - 18/05/2020. You can find more information about the derogation &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=EST" target="_blank"&gt;here&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Reservations &lt;br/&gt; &lt;br/&gt; Estonia made the following reservation  to the provisions of Article 1 of Protocol 1: &lt;br/&gt;&lt;br/&gt;  In accordance with Article 64 of the Convention, the Republic of Estonia declares that the provisions of Article 1 of the First Protocol shall not apply to the laws on property reform which regulate the restoration or compensation of property nationalised, confiscated, requisitioned, collectivised or otherwise unlawfully expropriated during the period of Soviet annexation; the restructuring of collectivised agriculture and privatisation of state owned property. The reservation concerns the Principles of the Property Reform Act (published in Riigi Teataja [State Gazette] 1991, 21, 257; RT I 1994, 38, 617; 40, 653; 51, 859; 94, 1609), the Land Reform Act (RT 1991, 34, 426; RT I 1995,, 10, 113), the Agricultural Reform Act (RT 1992, 10, 143; 36, 474; RT I 1994, 52, 880), the Privatisation Act (RT I 1993, 45, 639; 1994, 50, 846; 79, 1329; 83, 1448; 1995, 22, 327; 54, 881; 57, 979), the Dwelling Rooms Privatisation Act (RT I 1993, 23, 411; 1995, 44, 671; 57, 979; 1996, 2, 28), the Act on Evaluation and Compensation of Unlawfully Expropriated Property (RT I 1993, 30, 509; 1994, 8, 106; 51, 859; 54, 905; 1995, 29, 357), the Act on Evaluation of Collectivised Property (RT I 1993, 7, 104) and their wording being in force at the moment of the Ratification Act entered into force. &lt;br/&gt;&lt;br/&gt;&lt;br/&gt; Derogations &lt;br/&gt; Estonia temporarily derogated from certain of its obligations under the provisions of Article 1 of Protocol 1 during the emergency situation pursuant to the COVID-19 pandemic. Period covered by the derogation: 20/03/2020 - 18/05/2020. You can find more information about the derogation &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/009/declarations?p_auth=5IOZ28jl&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=EST" target="_blank"&gt;here&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estonia temporarily derogated from certain of its obligations under the provisions of Article 2 of Protocol 1 during the emergency situation pursuant to the COVID-19 pandemic. Period covered by the derogation: 20/03/2020 - 18/05/2020. You can find more information about the derogation &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/009/declarations?p_auth=5IOZ28jl&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=EST" target="_blank"&gt; here&lt;/a&gt;. </t>
+  </si>
+  <si>
+    <t>Estonia temporarily derogated from certain of its obligations under the provisions of Article 2 of Protocol 4 during the emergency situation pursuant to the COVID-19 pandemic. Period covered by the derogation: 20/03/2020 - 18/05/2020. You can find more information about the derogation &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/046/declarations?p_auth=5IOZ28jl&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=EST" target="_blank"&gt; here&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Georgia temporarily derogated from certain of its obligations under the provisions of Article 5 due to the COVID-19 pandemic. The derogation period started on 23/03/2020. (For updated information on the ongoing derogation, please &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=GEO" target="_blank"&gt;check here&lt;/a&gt;).</t>
+  </si>
+  <si>
+    <t>Georgia temporarily derogated from certain of its obligations under the provisions of Article 6 due to the COVID-19 pandemic. The derogation period started on 23/03/2020. (For updated information on the ongoing derogation, please  &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=GEO" target="_blank"&gt;check here&lt;/a&gt; ).</t>
+  </si>
+  <si>
+    <t>Georgia temporarily derogated from certain of its obligations under the provisions of Article 8 due to the COVID-19 pandemic. The derogation period started on 23/03/2020. For updated information on the ongoing derogation, please  &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=GEO" target="_blank"&gt;check here&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <r>
+      <t>Georgia temporarily derogated from certain of its obligations under the provisions of Article 8 due to the COVID-19 pandemic. The derogation period started on 23/03/2020. (For updated information on the ongoing derogation, please  &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=GEO" target="_blank"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">check </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>here&lt;/a&gt;).</t>
+    </r>
+  </si>
+  <si>
+    <t>Georgia triggered Article 15 during the following periods: 03/03/2006 - 16/03/2006 due to the H5N1 virus, 09/11/2007 - 16/11/2007 due to a coup d'Etat, and since 23/03/2020 onwards due to the COVID-19 pandemic.  For updated information on the ongoing derogation, please  &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=GEO" target="_blank"&gt;check here&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Reservations &lt;br/&gt;&lt;br/&gt; Georgia made the following reservation to the provisions of Article 1 of Protocol 1: &lt;br/&gt;1. Article 1 of the Protocol shall not apply to persons who have or will obtain status of “internally displaced persons” in accordance with “the Law of Georgia on Internally Displaced Persons” until the elimination of circumstances motivating the granting of this status (until the restoration of the territorial integrity of Georgia). In accordance with the aforementioned law, Georgia assumes responsibility to ensure the exercise of rights over property that exist on the place of permanent residence of internally displaced persons after the reasons mentioned in Article 1, paragraph 1, of this law have been eliminated.
+&lt;br/&gt; 
+2. Article 1 of the Protocol shall be applied to the operational sphere of “the Law of Georgia on the Ownership of Agricultural Land” in accordance with the requirements of Articles 4, 8, 15 and 19 of this Law.
+&lt;br/&gt; 
+3. Article 1 of the Protocol shall be applied within the limits of Articles 2 and 3 of the Law of Georgia on Transference into Private Property of the Non-Agricultural Lands Being in Possession of Natural Persons and Legal Persons of Private Law”.
+&lt;br/&gt; 
+4. Article 1 of the Protocol shall be applied within the limits of the “Law of Georgia on Privatisation of the State Property”. &lt;br/&gt; 
+5. With regard to the compensation of pecuniary assets placed on accounts of the former Georgian public-commercial banks, Article 1 of the Protocol shall be applied within the limits of the normative act adopted in pursuance of the Decree No. 258 of the President of Georgia of 2 July 2001.  &lt;br/&gt; &lt;br/&gt; Derogations &lt;br/&gt; Georgia has derogated from Article 1 of Protocol 1 during 03/03/2006 - 16/03/2006 and during the COVID-19 pandemic state of emergency which was instituted on 15/07/2020. &lt;br/&gt; &lt;br/&gt; Declarations &lt;br/&gt;Georgia made the following declaration upon ratidication of Protocol 1:&lt;br/&gt; Due to the existing situation in Abkhazia and Tskhinvali region, Georgian authorities are unable to undertake commitments concerning the respect and protection of the provisions of the Convention and its Additional Protocols on these territories. Georgia therefore declines its responsibility for violations of the provisions of the Protocol by the organs of self-proclaimed illegal forces on the territories of Abkhazia and Tskhinvali region until the possibility of realization of the full jurisdiction of Georgia is restored over these territories. The declaration is active since 07/06/2002.
+ &lt;br/&gt; &gt;br/&gt; &lt;br/&gt; Derogations &lt;br/&gt; &gt;br/&gt; Georgia temporarily derogated from certain of its obligations under the provisions of Article 1 of Protocol 1 due to the COVID-19 pandemic. The derogation period started on 23/03/2020. (For updated information on the ongoing derogation, please &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/009/declarations?p_auth=5IOZ28jl&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=GEO" target="_blank"&gt;check here&lt;/a&gt;).</t>
+  </si>
+  <si>
+    <t>Reservations &lt;br/&gt;&lt;br/&gt; Georgia made the following reservation to the provisions of Article 2 of Protocol 1: &lt;br/&gt; Georgia declares that it interprets Article 2 of the Protocol as not imposing on the State additional financial commitments relating to special educational establishments (with a specific philosophical or religious orientation) other than those provided by the legislation of Georgia.  &lt;br/&gt; &lt;br/&gt;&lt;br/&gt; Derogations &lt;br/&gt; Georgia temporarily derogated from certain of its obligations under the provisions of Article 2 of Protocol 1 during the COVID-19 pandemic state of emergency which was instituted on 15/07/2020. (For updated information on the ongoing derogation, please &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/009/declarations?p_auth=5IOZ28jl&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=GEO" target="_blank"&gt;check here&lt;/a&gt;). &lt;br/&gt; &lt;br/&gt;&lt;br/&gt; Declarations &lt;br/&gt; Georgia made the following declaration upon ratidication of Protocol 1: &lt;br/&gt; Due to the existing situation in Abkhazia and Tskhinvali region, Georgian authorities are unable to undertake commitments concerning the respect and protection of the provisions of the Convention and its Additional Protocols on these territories. Georgia therefore declines its responsibility for violations of the provisions of the Protocol by the organs of self-proclaimed illegal forces on the territories of Abkhazia and Tskhinvali region until the possibility of realization of the full jurisdiction of Georgia is restored over these territories.</t>
+  </si>
+  <si>
+    <t>Georgia temporarily derogated from certain of its obligations under the provisions of Article 2 of Protocol 4 due to the COVID-19 pandemic. The derogation period started on 23/03/2020. (For updated information on the ongoing derogation, please &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/046/declarations?p_auth=5IOZ28jl&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=GEO" target="_blank"&gt;check here&lt;/a&gt;).</t>
+  </si>
+  <si>
+    <t>Turkey declared state of emergency and triggered Article 15, thereby derogating from certain of its obligations under the European Convention on Human Rights, during the following periods: 28/02/1961 - 19/12/1961, 28/05/1963 - 29/07/1964, 19/06/1970 - 19/09/1970, 04/05/1971 - 26/09/1973, 24/07/1974 - 05/08/1975, 28/12/1978 - 19/07/1987, 06/08/1990 - 29/01/2002, 21/07/2016 - 19/07/2018. For more information please &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=TUR" target="_blank"&gt;check here&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Reservations &lt;br/&gt; &lt;br/&gt; Ukraine made the following reservations to the provisions of Article 5: &lt;br/&gt; The provisions of Article 5, paragraph 3, of the Convention for the Protection of Human Rights and Fundamental Freedoms of 1950 shall apply in the part that does not contradict paragraphs 50, 51, 52 and 53 of the Interim Disciplinary Statute of the Armed Forces of Ukraine approved by the Decree No 431 of the President of Ukraine dated 7 October 1993, concerning the imposition of arrest as a disciplinary sanction. &lt;br/&gt; &lt;br/&gt; (Period covered: 11/09/1997 - 29/06/2001) The provisions of Article 5, paragraph 1, of the Convention for the Protection of Human Rights and Fundamental Freedoms of 1950 shall apply in the part that does not contradict paragraph 13 of Chapter XV of the Transitional Provisions of the Constitution of Ukraine and Articles 106 and 157 of the Criminal Procedure Code of Ukraine concerning the detention of a person and the arrest warrant issued by the public prosecutor.  
+&lt;br/&gt; &lt;br/&gt; &lt;br/&gt;Derogations. &lt;br/&gt; &lt;br/&gt; Ukraine declared public emergency pursuant to the conflict in north-eastern Ukraine and derogated from certain of its obligations under the provisions of Article 5. Period covered: 09/06/2015 – ongoing. For further details regarding the state of emergency, please visit &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=U" target="_blank"&gt;this page&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reservations &lt;br/&gt; &lt;br/&gt; 
+Ukraine made the following reservations to the provisions of Article 6: &lt;br/&gt;
+Ukraine fully recognises on its territory the validity of Article 6, paragraph 3.d, of the Convention for the Protection of Human Rights and Fundamental Freedoms of 1950 in regard to the defendant's right to obtain the attendance and examination of witnesses (Articles 263 and 303 of the Criminal Procedure Code of Ukraine) and as regards the rights of the suspect and persons charged in pre-trial proceedings to submit petitions for the attendance and examination of witnesses and the confrontation with them in accordance with Articles 43, 431 and 142 of the above-mentioned Code.
+&lt;br/&gt; &lt;br/&gt; &lt;br/&gt;Derogations. &lt;br/&gt; &lt;br/&gt;  Ukraine declared public emergency pursuant to the conflict in north-eastern Ukraine and derogated from certain of its obligations under the provisions of  Article 6. Period covered: 09/06/2015 – ongoing. For further details regarding the state of emergency, please visit &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=U" target="_blank"&gt;this page&lt;/a&gt;. </t>
+  </si>
+  <si>
+    <t>Reservations &lt;br/&gt;&lt;br/&gt;
+Ukraine made the following reservation to the provisions of Article 8: &lt;br/&gt;  The provisions of Article 8 of the Convention for the Protection of Human Rights and Fundamental Freedoms of 1950 shall apply in the part that does not contradict paragraph 13 of Chapter XV "Transitional Provisions" of the Constitution of Ukraine and Articles 177 and 190 of the Criminal Procedure Code of Ukraine concerning warrants for arrest and search warrants issued by the public prosecutor. Period covered: 11/09/1997 - 28/06/2001.
+&lt;br/&gt;&lt;br/&gt; &lt;br/&gt;Derogations. &lt;br/&gt;&lt;br/&gt; Ukraine declared public emergency pursuant to the conflict in north-eastern Ukraine and derogated from certain of its obligations under the provisions of Article 8. Period covered: 09/06/2015 – ongoing. For further details regarding the state of emergency, please visit &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=U" target="_blank"&gt;this page&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ukraine declared public emergency pursuant to the conflict in north-eastern Ukraine and derogated from certain of its obligations under the provisions of Article 13. Period covered: 09/06/2015 – ongoing. For further details regarding the state of emergency, please visit &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=U" target="_blank"&gt;this page&lt;/a&gt;. </t>
+  </si>
+  <si>
+    <t>Ukraine declared public emergency pursuant to the conflict in north-eastern Ukraine and triggered Article 15 from 09/06/2015 onwards. For further details regarding the state of emergency, please visit &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=GM3ksCqs&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=U" target="_blank"&gt;this page&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ukraine declared public emergency pursuant to the conflict in north-eastern Ukraine and derogated from certain of its obligations under the provisions of Article 2 of Protocol 4. . Period covered: 09/06/2015 – ongoing. Please follow &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=i2TjEjny&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=U&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10" target="_blank"&gt;this link&lt;/a&gt; for further details.  </t>
+  </si>
+  <si>
+    <t>Derogations &lt;br/&gt; &lt;br/&gt; The United Kingdom triggered Article 15 during the following periods: [derogations before 01/09/1966, though existing, are not mentioned] 01/09/1966 - 30/11/1967, 25/09/1969 - 22/08/1984, 23/12/1988 - 05/05/2006, when certain provisions of the European Convention on Human Rights are derogated from. For further details, see &lt;a href="https://www.coe.int/en/web/conventions/search-on-treaties/-/conventions/treaty/005/declarations?p_auth=i2TjEjny&amp;_coeconventions_WAR_coeconventionsportlet_enVigueur=false&amp;_coeconventions_WAR_coeconventionsportlet_searchBy=state&amp;_coeconventions_WAR_coeconventionsportlet_codePays=UK&amp;_coeconventions_WAR_coeconventionsportlet_codeNature=10" target="_blank"&gt;here&lt;/a&gt;.     Territorial application &lt;br/&gt; &lt;br/&gt;
 United Kingdom and Northern Ireland’s government has extended the territorial application as follows of the European Convention on Human Rights as follows: &lt;br/&gt;&lt;br/&gt;
 Territorial extension accepted on a permanent basis as from 14 January 2001: Bailiwick of Jersey. &lt;br/&gt;
 Territorial extension accepted on a permanent basis as from 1 June 2003: Isle of Man. &lt;br/&gt;
@@ -1315,7 +1334,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1343,6 +1362,12 @@
       <family val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <name val="Garamond"/>
       <family val="1"/>
@@ -13279,8 +13304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81983450-F4B6-404D-BA41-2CE61199491F}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13289,7 +13314,7 @@
     <col min="2" max="2" width="14.44140625" style="15"/>
     <col min="3" max="3" width="13.5546875" style="15" customWidth="1"/>
     <col min="4" max="4" width="5.44140625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="42.88671875" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.33203125" style="15" customWidth="1"/>
     <col min="7" max="16384" width="14.44140625" style="15"/>
   </cols>
@@ -13415,7 +13440,7 @@
         <v>97</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>15</v>
@@ -14249,7 +14274,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -14846,7 +14871,7 @@
         <v>97</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="F28" s="16" t="s">
         <v>59</v>
@@ -15331,7 +15356,7 @@
         <v>97</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>13</v>
@@ -15354,7 +15379,7 @@
         <v>97</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>15</v>
@@ -16845,7 +16870,7 @@
         <v>97</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="F31" s="16" t="s">
         <v>65</v>
@@ -16868,7 +16893,7 @@
         <v>97</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="F32" s="16" t="s">
         <v>67</v>
@@ -16891,7 +16916,7 @@
         <v>97</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="F33" s="16" t="s">
         <v>69</v>
@@ -16914,7 +16939,7 @@
         <v>97</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="F34" s="16" t="s">
         <v>96</v>
@@ -16937,7 +16962,7 @@
         <v>97</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="F35" s="16" t="s">
         <v>73</v>
@@ -16979,7 +17004,7 @@
         <v>97</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="F37" s="16" t="s">
         <v>77</v>
@@ -17162,8 +17187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA61694C-FF1D-47C3-8B80-CE4DF79BE172}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -17172,7 +17197,7 @@
     <col min="2" max="2" width="14.44140625" style="15"/>
     <col min="3" max="3" width="11.6640625" style="15" customWidth="1"/>
     <col min="4" max="4" width="3.88671875" style="15" customWidth="1"/>
-    <col min="5" max="5" width="33.77734375" style="15" customWidth="1"/>
+    <col min="5" max="5" width="255.77734375" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.33203125" style="15" customWidth="1"/>
     <col min="7" max="16384" width="14.44140625" style="15"/>
   </cols>
@@ -17277,7 +17302,7 @@
         <v>97</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>200</v>
+        <v>312</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>13</v>
@@ -17300,7 +17325,7 @@
         <v>97</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>206</v>
+        <v>313</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>15</v>
@@ -17344,7 +17369,7 @@
         <v>97</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>201</v>
+        <v>314</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>19</v>
@@ -17409,7 +17434,7 @@
         <v>97</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>202</v>
+        <v>315</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>25</v>
@@ -17495,7 +17520,7 @@
         <v>97</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>330</v>
+        <v>295</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>33</v>
@@ -17644,7 +17669,7 @@
         <v>97</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>205</v>
+        <v>316</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>47</v>
@@ -17667,7 +17692,7 @@
         <v>97</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>204</v>
+        <v>317</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>49</v>
@@ -17732,7 +17757,7 @@
         <v>97</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>203</v>
+        <v>318</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>55</v>
@@ -18287,7 +18312,7 @@
         <v>97</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>15</v>
@@ -19172,7 +19197,7 @@
         <v>97</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>7</v>
@@ -19195,7 +19220,7 @@
         <v>97</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>9</v>
@@ -19218,7 +19243,7 @@
         <v>97</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>11</v>
@@ -19241,7 +19266,7 @@
         <v>97</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>13</v>
@@ -19264,7 +19289,7 @@
         <v>97</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>15</v>
@@ -19287,7 +19312,7 @@
         <v>97</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>17</v>
@@ -19310,7 +19335,7 @@
         <v>97</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>19</v>
@@ -19333,7 +19358,7 @@
         <v>97</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>21</v>
@@ -19356,7 +19381,7 @@
         <v>97</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>23</v>
@@ -19379,7 +19404,7 @@
         <v>97</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>25</v>
@@ -19402,7 +19427,7 @@
         <v>97</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>27</v>
@@ -19425,7 +19450,7 @@
         <v>97</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>29</v>
@@ -19448,7 +19473,7 @@
         <v>97</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F14" s="16" t="s">
         <v>31</v>
@@ -19471,7 +19496,7 @@
         <v>97</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>329</v>
+        <v>294</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>33</v>
@@ -19494,7 +19519,7 @@
         <v>97</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>35</v>
@@ -19517,7 +19542,7 @@
         <v>97</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>37</v>
@@ -19540,7 +19565,7 @@
         <v>97</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>39</v>
@@ -19563,7 +19588,7 @@
         <v>97</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F19" s="16" t="s">
         <v>41</v>
@@ -19586,7 +19611,7 @@
         <v>97</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>43</v>
@@ -19609,7 +19634,7 @@
         <v>97</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>45</v>
@@ -19632,7 +19657,7 @@
         <v>97</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>47</v>
@@ -19655,7 +19680,7 @@
         <v>97</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>49</v>
@@ -19678,7 +19703,7 @@
         <v>97</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="F24" s="16" t="s">
         <v>51</v>
@@ -19701,7 +19726,7 @@
         <v>97</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="F25" s="16" t="s">
         <v>53</v>
@@ -19724,7 +19749,7 @@
         <v>97</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>55</v>
@@ -19747,7 +19772,7 @@
         <v>97</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="F27" s="16" t="s">
         <v>57</v>
@@ -19770,7 +19795,7 @@
         <v>97</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="F28" s="16" t="s">
         <v>59</v>
@@ -19835,7 +19860,7 @@
         <v>97</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="F31" s="16" t="s">
         <v>65</v>
@@ -19858,7 +19883,7 @@
         <v>97</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="F32" s="16" t="s">
         <v>67</v>
@@ -19881,7 +19906,7 @@
         <v>97</v>
       </c>
       <c r="E33" s="26" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="F33" s="16" t="s">
         <v>69</v>
@@ -19904,7 +19929,7 @@
         <v>97</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="F34" s="16" t="s">
         <v>96</v>
@@ -19927,7 +19952,7 @@
         <v>97</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="F35" s="16" t="s">
         <v>73</v>
@@ -20004,7 +20029,7 @@
         <v>97</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F39" s="16" t="s">
         <v>79</v>
@@ -20027,7 +20052,7 @@
         <v>97</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F40" s="16" t="s">
         <v>81</v>
@@ -20050,7 +20075,7 @@
         <v>97</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F41" s="16" t="s">
         <v>83</v>
@@ -20073,7 +20098,7 @@
         <v>97</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F42" s="16" t="s">
         <v>85</v>
@@ -20096,7 +20121,7 @@
         <v>97</v>
       </c>
       <c r="E43" s="26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F43" s="16" t="s">
         <v>87</v>
@@ -20119,7 +20144,7 @@
         <v>97</v>
       </c>
       <c r="E44" s="26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F44" s="16" t="s">
         <v>89</v>
@@ -20142,7 +20167,7 @@
         <v>97</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="F45" s="16" t="s">
         <v>91</v>
@@ -20164,8 +20189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F650EE95-76AA-4239-AD18-5B10D171F38D}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -20279,7 +20304,7 @@
         <v>97</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>221</v>
+        <v>319</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>13</v>
@@ -20302,7 +20327,7 @@
         <v>97</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>222</v>
+        <v>320</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>15</v>
@@ -20346,7 +20371,7 @@
         <v>97</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>19</v>
@@ -20411,7 +20436,7 @@
         <v>97</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>220</v>
+        <v>322</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>25</v>
@@ -20497,7 +20522,7 @@
         <v>97</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>33</v>
@@ -20646,7 +20671,7 @@
         <v>97</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>225</v>
+        <v>324</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>47</v>
@@ -20669,7 +20694,7 @@
         <v>97</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>226</v>
+        <v>325</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>49</v>
@@ -20692,7 +20717,7 @@
         <v>97</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
       <c r="F24" s="16" t="s">
         <v>51</v>
@@ -20736,7 +20761,7 @@
         <v>97</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>224</v>
+        <v>326</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>55</v>
@@ -20948,7 +20973,7 @@
         <v>97</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>227</v>
+        <v>201</v>
       </c>
       <c r="F36" s="16" t="s">
         <v>75</v>
@@ -20971,7 +20996,7 @@
         <v>97</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>228</v>
+        <v>202</v>
       </c>
       <c r="F37" s="16" t="s">
         <v>77</v>
@@ -21143,8 +21168,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -21643,7 +21669,7 @@
         <v>97</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>229</v>
+        <v>203</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>49</v>
@@ -21771,7 +21797,7 @@
         <v>97</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
       <c r="F29" s="16" t="s">
         <v>61</v>
@@ -21794,7 +21820,7 @@
         <v>97</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
       <c r="F30" s="16" t="s">
         <v>95</v>
@@ -21838,7 +21864,7 @@
         <v>101</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
       <c r="F32" s="16" t="s">
         <v>67</v>
@@ -21861,7 +21887,7 @@
         <v>101</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>232</v>
+        <v>206</v>
       </c>
       <c r="F33" s="16" t="s">
         <v>69</v>
@@ -21884,7 +21910,7 @@
         <v>101</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>233</v>
+        <v>207</v>
       </c>
       <c r="F34" s="16" t="s">
         <v>96</v>
@@ -23088,8 +23114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF169478-4C06-4529-B0D9-8A1E24BB8D4E}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -23098,7 +23124,7 @@
     <col min="2" max="2" width="14.44140625" style="15"/>
     <col min="3" max="3" width="14.44140625" style="19"/>
     <col min="4" max="4" width="5.21875" style="19" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="255.77734375" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.33203125" style="15" customWidth="1"/>
     <col min="7" max="16384" width="14.44140625" style="15"/>
   </cols>
@@ -23266,7 +23292,7 @@
         <v>97</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>19</v>
@@ -23331,7 +23357,7 @@
         <v>97</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>25</v>
@@ -23417,7 +23443,7 @@
         <v>97</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>332</v>
+        <v>296</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>33</v>
@@ -23566,7 +23592,7 @@
         <v>97</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>47</v>
@@ -23589,7 +23615,7 @@
         <v>97</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>49</v>
@@ -23656,7 +23682,7 @@
         <v>97</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>55</v>
@@ -26140,7 +26166,7 @@
         <v>97</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>234</v>
+        <v>208</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>15</v>
@@ -26499,7 +26525,7 @@
         <v>97</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>235</v>
+        <v>209</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>49</v>
@@ -26585,7 +26611,7 @@
         <v>97</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>236</v>
+        <v>210</v>
       </c>
       <c r="F27" s="16" t="s">
         <v>57</v>
@@ -27554,7 +27580,7 @@
         <v>97</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>237</v>
+        <v>211</v>
       </c>
       <c r="F27" s="16" t="s">
         <v>57</v>
@@ -27661,7 +27687,7 @@
         <v>97</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>238</v>
+        <v>212</v>
       </c>
       <c r="F32" s="16" t="s">
         <v>67</v>
@@ -27684,7 +27710,7 @@
         <v>97</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>239</v>
+        <v>213</v>
       </c>
       <c r="F33" s="16" t="s">
         <v>69</v>
@@ -27707,7 +27733,7 @@
         <v>97</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>240</v>
+        <v>214</v>
       </c>
       <c r="F34" s="16" t="s">
         <v>96</v>
@@ -28131,7 +28157,7 @@
         <v>97</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>241</v>
+        <v>215</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>19</v>
@@ -28196,7 +28222,7 @@
         <v>97</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>25</v>
@@ -28282,7 +28308,7 @@
         <v>97</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>326</v>
+        <v>293</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>33</v>
@@ -28431,7 +28457,7 @@
         <v>97</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>47</v>
@@ -28454,7 +28480,7 @@
         <v>97</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>49</v>
@@ -28519,7 +28545,7 @@
         <v>97</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>55</v>
@@ -28981,7 +29007,7 @@
         <v>97</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>246</v>
+        <v>220</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>7</v>
@@ -29067,7 +29093,7 @@
         <v>97</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>247</v>
+        <v>221</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>15</v>
@@ -29111,7 +29137,7 @@
         <v>97</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>19</v>
@@ -29617,7 +29643,7 @@
         <v>97</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>248</v>
+        <v>222</v>
       </c>
       <c r="F32" s="16" t="s">
         <v>67</v>
@@ -30019,7 +30045,7 @@
         <v>97</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>249</v>
+        <v>223</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>13</v>
@@ -31344,7 +31370,7 @@
         <v>97</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>250</v>
+        <v>224</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>47</v>
@@ -31619,7 +31645,7 @@
         <v>97</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>251</v>
+        <v>225</v>
       </c>
       <c r="F35" s="16" t="s">
         <v>73</v>
@@ -31895,7 +31921,7 @@
         <v>97</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>252</v>
+        <v>226</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>7</v>
@@ -31981,7 +32007,7 @@
         <v>97</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>253</v>
+        <v>227</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>15</v>
@@ -32067,7 +32093,7 @@
         <v>97</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>254</v>
+        <v>228</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>23</v>
@@ -32342,7 +32368,7 @@
         <v>97</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>255</v>
+        <v>229</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>49</v>
@@ -32871,7 +32897,7 @@
         <v>97</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>7</v>
@@ -32894,7 +32920,7 @@
         <v>97</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>9</v>
@@ -32917,7 +32943,7 @@
         <v>97</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>11</v>
@@ -32940,7 +32966,7 @@
         <v>97</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>13</v>
@@ -32963,7 +32989,7 @@
         <v>97</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>15</v>
@@ -32986,7 +33012,7 @@
         <v>97</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>258</v>
+        <v>232</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>17</v>
@@ -33009,7 +33035,7 @@
         <v>97</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>19</v>
@@ -33055,7 +33081,7 @@
         <v>97</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>260</v>
+        <v>234</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>23</v>
@@ -33078,7 +33104,7 @@
         <v>97</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>261</v>
+        <v>235</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>25</v>
@@ -33124,7 +33150,7 @@
         <v>97</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>262</v>
+        <v>236</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>29</v>
@@ -33147,7 +33173,7 @@
         <v>97</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F14" s="16" t="s">
         <v>31</v>
@@ -33170,7 +33196,7 @@
         <v>97</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>33</v>
@@ -33193,7 +33219,7 @@
         <v>97</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>35</v>
@@ -33216,7 +33242,7 @@
         <v>97</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>37</v>
@@ -33239,7 +33265,7 @@
         <v>97</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>39</v>
@@ -33262,7 +33288,7 @@
         <v>97</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F19" s="16" t="s">
         <v>41</v>
@@ -33285,7 +33311,7 @@
         <v>97</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>43</v>
@@ -33308,7 +33334,7 @@
         <v>97</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>45</v>
@@ -33415,7 +33441,7 @@
         <v>97</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>263</v>
+        <v>237</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>55</v>
@@ -33543,7 +33569,7 @@
         <v>97</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>264</v>
+        <v>238</v>
       </c>
       <c r="F32" s="16" t="s">
         <v>67</v>
@@ -33683,7 +33709,7 @@
         <v>97</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F39" s="16" t="s">
         <v>79</v>
@@ -33706,7 +33732,7 @@
         <v>97</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F40" s="16" t="s">
         <v>81</v>
@@ -33729,7 +33755,7 @@
         <v>97</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F41" s="16" t="s">
         <v>83</v>
@@ -33752,7 +33778,7 @@
         <v>97</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F42" s="16" t="s">
         <v>85</v>
@@ -33775,7 +33801,7 @@
         <v>97</v>
       </c>
       <c r="E43" s="26" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F43" s="16" t="s">
         <v>87</v>
@@ -33798,7 +33824,7 @@
         <v>97</v>
       </c>
       <c r="E44" s="26" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F44" s="16" t="s">
         <v>89</v>
@@ -33821,7 +33847,7 @@
         <v>97</v>
       </c>
       <c r="E45" s="26" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F45" s="16" t="s">
         <v>91</v>
@@ -33842,8 +33868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC2FCF58-5775-4882-801F-E0EE601209F3}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="E10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -33852,7 +33878,7 @@
     <col min="2" max="2" width="14.44140625" style="15"/>
     <col min="3" max="3" width="11" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.5546875" style="15" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="255.77734375" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.33203125" style="15" customWidth="1"/>
     <col min="7" max="16384" width="14.44140625" style="15"/>
   </cols>
@@ -34933,7 +34959,7 @@
         <v>97</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>265</v>
+        <v>239</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>13</v>
@@ -34956,7 +34982,7 @@
         <v>97</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>266</v>
+        <v>240</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>15</v>
@@ -35790,7 +35816,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -35842,7 +35868,7 @@
         <v>97</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>7</v>
@@ -35865,7 +35891,7 @@
         <v>97</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>9</v>
@@ -35888,7 +35914,7 @@
         <v>97</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>11</v>
@@ -35911,7 +35937,7 @@
         <v>97</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>13</v>
@@ -35934,7 +35960,7 @@
         <v>97</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>15</v>
@@ -35957,7 +35983,7 @@
         <v>97</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>17</v>
@@ -35980,7 +36006,7 @@
         <v>97</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>19</v>
@@ -36003,7 +36029,7 @@
         <v>97</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>21</v>
@@ -36026,7 +36052,7 @@
         <v>97</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>23</v>
@@ -36049,7 +36075,7 @@
         <v>97</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>25</v>
@@ -36072,7 +36098,7 @@
         <v>97</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>27</v>
@@ -36095,7 +36121,7 @@
         <v>97</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>29</v>
@@ -36118,7 +36144,7 @@
         <v>97</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="F14" s="16" t="s">
         <v>31</v>
@@ -36141,7 +36167,7 @@
         <v>97</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>33</v>
@@ -36164,7 +36190,7 @@
         <v>97</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>35</v>
@@ -36187,7 +36213,7 @@
         <v>97</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>37</v>
@@ -36210,7 +36236,7 @@
         <v>97</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>39</v>
@@ -36233,7 +36259,7 @@
         <v>97</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="F19" s="16" t="s">
         <v>41</v>
@@ -36256,7 +36282,7 @@
         <v>97</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>43</v>
@@ -36279,7 +36305,7 @@
         <v>97</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>45</v>
@@ -36302,7 +36328,7 @@
         <v>97</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>309</v>
+        <v>283</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>47</v>
@@ -36325,7 +36351,7 @@
         <v>97</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>310</v>
+        <v>284</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>49</v>
@@ -36348,7 +36374,7 @@
         <v>97</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>268</v>
+        <v>242</v>
       </c>
       <c r="F24" s="16" t="s">
         <v>51</v>
@@ -36392,7 +36418,7 @@
         <v>97</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>270</v>
+        <v>244</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>55</v>
@@ -36415,7 +36441,7 @@
         <v>97</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>271</v>
+        <v>245</v>
       </c>
       <c r="F27" s="16" t="s">
         <v>57</v>
@@ -36459,7 +36485,7 @@
         <v>97</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
       <c r="F29" s="16" t="s">
         <v>61</v>
@@ -36482,7 +36508,7 @@
         <v>97</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
       <c r="F30" s="16" t="s">
         <v>95</v>
@@ -36526,7 +36552,7 @@
         <v>101</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>274</v>
+        <v>248</v>
       </c>
       <c r="F32" s="16" t="s">
         <v>67</v>
@@ -36612,7 +36638,7 @@
         <v>97</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>272</v>
+        <v>246</v>
       </c>
       <c r="F36" s="16" t="s">
         <v>75</v>
@@ -36635,7 +36661,7 @@
         <v>97</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>273</v>
+        <v>247</v>
       </c>
       <c r="F37" s="16" t="s">
         <v>77</v>
@@ -36672,7 +36698,7 @@
         <v>97</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>269</v>
+        <v>243</v>
       </c>
       <c r="F39" s="16" t="s">
         <v>79</v>
@@ -36695,7 +36721,7 @@
         <v>97</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>269</v>
+        <v>243</v>
       </c>
       <c r="F40" s="16" t="s">
         <v>81</v>
@@ -36718,7 +36744,7 @@
         <v>97</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>269</v>
+        <v>243</v>
       </c>
       <c r="F41" s="16" t="s">
         <v>83</v>
@@ -36741,7 +36767,7 @@
         <v>97</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>269</v>
+        <v>243</v>
       </c>
       <c r="F42" s="16" t="s">
         <v>85</v>
@@ -36764,7 +36790,7 @@
         <v>97</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>269</v>
+        <v>243</v>
       </c>
       <c r="F43" s="16" t="s">
         <v>87</v>
@@ -36787,7 +36813,7 @@
         <v>97</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>269</v>
+        <v>243</v>
       </c>
       <c r="F44" s="16" t="s">
         <v>89</v>
@@ -36810,7 +36836,7 @@
         <v>97</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>269</v>
+        <v>243</v>
       </c>
       <c r="F45" s="16" t="s">
         <v>91</v>
@@ -37010,7 +37036,7 @@
         <v>97</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>275</v>
+        <v>249</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>19</v>
@@ -37075,7 +37101,7 @@
         <v>97</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>276</v>
+        <v>250</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>25</v>
@@ -37161,7 +37187,7 @@
         <v>97</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>325</v>
+        <v>292</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>33</v>
@@ -37331,7 +37357,7 @@
         <v>97</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>277</v>
+        <v>251</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>49</v>
@@ -37396,7 +37422,7 @@
         <v>97</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>278</v>
+        <v>252</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>55</v>
@@ -39859,7 +39885,7 @@
         <v>97</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>280</v>
+        <v>254</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>13</v>
@@ -39903,7 +39929,7 @@
         <v>97</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>279</v>
+        <v>253</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>17</v>
@@ -40430,7 +40456,7 @@
         <v>97</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>281</v>
+        <v>255</v>
       </c>
       <c r="F32" s="16" t="s">
         <v>67</v>
@@ -40474,7 +40500,7 @@
         <v>97</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>282</v>
+        <v>256</v>
       </c>
       <c r="F34" s="16" t="s">
         <v>96</v>
@@ -40772,7 +40798,7 @@
         <v>97</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>7</v>
@@ -40795,7 +40821,7 @@
         <v>97</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>9</v>
@@ -40818,7 +40844,7 @@
         <v>97</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>284</v>
+        <v>258</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>11</v>
@@ -40864,7 +40890,7 @@
         <v>97</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>15</v>
@@ -40887,7 +40913,7 @@
         <v>97</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>17</v>
@@ -40910,7 +40936,7 @@
         <v>97</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>19</v>
@@ -40933,7 +40959,7 @@
         <v>97</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>21</v>
@@ -40956,7 +40982,7 @@
         <v>97</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>23</v>
@@ -40979,7 +41005,7 @@
         <v>97</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>285</v>
+        <v>259</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>25</v>
@@ -41002,7 +41028,7 @@
         <v>97</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>27</v>
@@ -41025,7 +41051,7 @@
         <v>97</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>29</v>
@@ -41048,7 +41074,7 @@
         <v>97</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F14" s="16" t="s">
         <v>31</v>
@@ -41071,7 +41097,7 @@
         <v>97</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>324</v>
+        <v>291</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>33</v>
@@ -41094,7 +41120,7 @@
         <v>97</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>35</v>
@@ -41117,7 +41143,7 @@
         <v>97</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>37</v>
@@ -41140,7 +41166,7 @@
         <v>97</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>39</v>
@@ -41163,7 +41189,7 @@
         <v>97</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F19" s="16" t="s">
         <v>41</v>
@@ -41186,7 +41212,7 @@
         <v>97</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>43</v>
@@ -41209,7 +41235,7 @@
         <v>97</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>45</v>
@@ -41253,7 +41279,7 @@
         <v>97</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>288</v>
+        <v>262</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>49</v>
@@ -41318,7 +41344,7 @@
         <v>97</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>286</v>
+        <v>260</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>55</v>
@@ -41551,7 +41577,7 @@
         <v>97</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>287</v>
+        <v>261</v>
       </c>
       <c r="F37" s="16" t="s">
         <v>77</v>
@@ -41588,7 +41614,7 @@
         <v>97</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F39" s="16" t="s">
         <v>79</v>
@@ -41611,7 +41637,7 @@
         <v>97</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F40" s="16" t="s">
         <v>81</v>
@@ -41634,7 +41660,7 @@
         <v>97</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F41" s="16" t="s">
         <v>83</v>
@@ -41657,7 +41683,7 @@
         <v>97</v>
       </c>
       <c r="E42" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F42" s="16" t="s">
         <v>85</v>
@@ -41680,7 +41706,7 @@
         <v>97</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F43" s="16" t="s">
         <v>87</v>
@@ -41703,7 +41729,7 @@
         <v>97</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F44" s="16" t="s">
         <v>89</v>
@@ -41726,7 +41752,7 @@
         <v>97</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="F45" s="16" t="s">
         <v>91</v>
@@ -41747,8 +41773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D773F7-E8C2-491B-8576-E9C9A6FDFB0A}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -41863,7 +41889,7 @@
         <v>97</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>289</v>
+        <v>263</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>13</v>
@@ -42075,7 +42101,7 @@
         <v>97</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>323</v>
+        <v>290</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>33</v>
@@ -42245,7 +42271,7 @@
         <v>97</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>290</v>
+        <v>264</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>49</v>
@@ -42837,7 +42863,7 @@
         <v>97</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>291</v>
+        <v>265</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>13</v>
@@ -43931,7 +43957,7 @@
         <v>97</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>292</v>
+        <v>266</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>25</v>
@@ -44017,7 +44043,7 @@
         <v>97</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>322</v>
+        <v>289</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>33</v>
@@ -44166,7 +44192,7 @@
         <v>97</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>293</v>
+        <v>267</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>47</v>
@@ -44399,7 +44425,7 @@
         <v>97</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>294</v>
+        <v>268</v>
       </c>
       <c r="F33" s="16" t="s">
         <v>69</v>
@@ -44665,14 +44691,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778548A8-314B-45F7-A896-B2962CB86904}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.33203125" style="15" customWidth="1"/>
-    <col min="2" max="16384" width="12.21875" style="15"/>
+    <col min="2" max="4" width="12.21875" style="15"/>
+    <col min="5" max="5" width="255.77734375" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="12.21875" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -44840,7 +44868,7 @@
         <v>97</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>179</v>
+        <v>298</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>19</v>
@@ -44884,7 +44912,7 @@
         <v>97</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>180</v>
+        <v>299</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>23</v>
@@ -44907,7 +44935,7 @@
         <v>97</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>181</v>
+        <v>300</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>25</v>
@@ -44993,7 +45021,7 @@
         <v>97</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>331</v>
+        <v>301</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>33</v>
@@ -45142,7 +45170,7 @@
         <v>97</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>182</v>
+        <v>302</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>47</v>
@@ -45228,7 +45256,7 @@
         <v>97</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>183</v>
+        <v>303</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>55</v>
@@ -45757,7 +45785,7 @@
         <v>97</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>296</v>
+        <v>270</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>13</v>
@@ -45780,7 +45808,7 @@
         <v>97</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>295</v>
+        <v>269</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>15</v>
@@ -45929,7 +45957,7 @@
         <v>97</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>297</v>
+        <v>271</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>29</v>
@@ -45973,7 +46001,7 @@
         <v>97</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>321</v>
+        <v>288</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>33</v>
@@ -46734,7 +46762,7 @@
         <v>97</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>298</v>
+        <v>272</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>13</v>
@@ -46757,7 +46785,7 @@
         <v>97</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>299</v>
+        <v>273</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>15</v>
@@ -48674,7 +48702,7 @@
         <v>97</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>300</v>
+        <v>274</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>13</v>
@@ -48697,7 +48725,7 @@
         <v>97</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>301</v>
+        <v>275</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>15</v>
@@ -48783,7 +48811,7 @@
         <v>97</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>302</v>
+        <v>276</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>23</v>
@@ -48892,7 +48920,7 @@
         <v>97</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>303</v>
+        <v>277</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>33</v>
@@ -49541,7 +49569,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -50034,7 +50062,7 @@
         <v>97</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>304</v>
+        <v>278</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>49</v>
@@ -50204,7 +50232,7 @@
         <v>97</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>305</v>
+        <v>279</v>
       </c>
       <c r="F31" s="16" t="s">
         <v>65</v>
@@ -51164,7 +51192,7 @@
         <v>97</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>306</v>
+        <v>280</v>
       </c>
       <c r="F31" s="16" t="s">
         <v>65</v>
@@ -51250,7 +51278,7 @@
         <v>97</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>307</v>
+        <v>281</v>
       </c>
       <c r="F35" s="16" t="s">
         <v>73</v>
@@ -51473,8 +51501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63E2771A-6B12-4E28-8821-D65CC8355162}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -51799,7 +51827,7 @@
         <v>97</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>33</v>
@@ -51969,7 +51997,7 @@
         <v>97</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>311</v>
+        <v>285</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>49</v>
@@ -52446,7 +52474,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -52561,7 +52589,7 @@
         <v>97</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>314</v>
+        <v>328</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>13</v>
@@ -52584,7 +52612,7 @@
         <v>97</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>15</v>
@@ -52628,7 +52656,7 @@
         <v>97</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>313</v>
+        <v>330</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>19</v>
@@ -52735,7 +52763,7 @@
         <v>97</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>312</v>
+        <v>331</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>29</v>
@@ -52779,7 +52807,7 @@
         <v>97</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>33</v>
@@ -53012,7 +53040,7 @@
         <v>97</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>316</v>
+        <v>333</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>55</v>
@@ -53063,7 +53091,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A29" s="16">
         <v>28</v>
       </c>
@@ -53076,8 +53104,8 @@
       <c r="D29" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="E29" s="16" t="s">
-        <v>317</v>
+      <c r="E29" s="20" t="s">
+        <v>286</v>
       </c>
       <c r="F29" s="16" t="s">
         <v>61</v>
@@ -53086,7 +53114,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A30" s="16">
         <v>29</v>
       </c>
@@ -53099,8 +53127,8 @@
       <c r="D30" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="E30" s="16" t="s">
-        <v>318</v>
+      <c r="E30" s="20" t="s">
+        <v>287</v>
       </c>
       <c r="F30" s="16" t="s">
         <v>95</v>
@@ -53429,8 +53457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E254CF-4207-4E4D-9ACD-7DE444A37AFB}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -53482,7 +53510,7 @@
         <v>97</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>7</v>
@@ -53505,7 +53533,7 @@
         <v>97</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>9</v>
@@ -53528,7 +53556,7 @@
         <v>97</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>11</v>
@@ -53551,7 +53579,7 @@
         <v>97</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>13</v>
@@ -53574,7 +53602,7 @@
         <v>97</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>15</v>
@@ -53597,7 +53625,7 @@
         <v>97</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>17</v>
@@ -53620,7 +53648,7 @@
         <v>97</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>19</v>
@@ -53643,7 +53671,7 @@
         <v>97</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>21</v>
@@ -53666,7 +53694,7 @@
         <v>97</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>23</v>
@@ -53689,7 +53717,7 @@
         <v>97</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>25</v>
@@ -53712,7 +53740,7 @@
         <v>97</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>27</v>
@@ -53735,7 +53763,7 @@
         <v>97</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>29</v>
@@ -53758,7 +53786,7 @@
         <v>97</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>31</v>
@@ -53804,7 +53832,7 @@
         <v>97</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>35</v>
@@ -53827,7 +53855,7 @@
         <v>97</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>37</v>
@@ -53850,7 +53878,7 @@
         <v>97</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>39</v>
@@ -53873,7 +53901,7 @@
         <v>97</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>41</v>
@@ -53896,7 +53924,7 @@
         <v>97</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>43</v>
@@ -53919,7 +53947,7 @@
         <v>97</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>45</v>
@@ -54288,7 +54316,7 @@
         <v>97</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>79</v>
@@ -54311,7 +54339,7 @@
         <v>97</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>81</v>
@@ -54334,7 +54362,7 @@
         <v>97</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>83</v>
@@ -54357,7 +54385,7 @@
         <v>97</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>85</v>
@@ -54380,7 +54408,7 @@
         <v>97</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>87</v>
@@ -54403,7 +54431,7 @@
         <v>97</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>89</v>
@@ -54424,7 +54452,7 @@
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="7" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>91</v>
@@ -54446,8 +54474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240184EA-956A-4854-ADA9-0C723ADA9B75}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -54456,7 +54484,7 @@
     <col min="2" max="2" width="14.44140625" style="15"/>
     <col min="3" max="3" width="13.6640625" style="15" customWidth="1"/>
     <col min="4" max="4" width="4.109375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="27.5546875" style="15" customWidth="1"/>
+    <col min="5" max="5" width="255.77734375" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.33203125" style="15" customWidth="1"/>
     <col min="7" max="16384" width="14.44140625" style="15"/>
   </cols>
@@ -55427,8 +55455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB552A6E-41CE-4026-B774-A5877E62DE31}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -55437,7 +55465,7 @@
     <col min="2" max="2" width="14.44140625" style="15"/>
     <col min="3" max="3" width="12" style="15" customWidth="1"/>
     <col min="4" max="4" width="5.33203125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="30.88671875" style="15" customWidth="1"/>
+    <col min="5" max="5" width="255.77734375" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.33203125" style="15" customWidth="1"/>
     <col min="7" max="16384" width="14.44140625" style="15"/>
   </cols>
@@ -55548,7 +55576,7 @@
         <v>97</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>173</v>
+        <v>304</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>13</v>
@@ -55571,7 +55599,7 @@
         <v>97</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>187</v>
+        <v>305</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>15</v>
@@ -55617,7 +55645,7 @@
         <v>97</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>172</v>
+        <v>306</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>19</v>
@@ -55663,7 +55691,7 @@
         <v>97</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>186</v>
+        <v>307</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>23</v>
@@ -55686,7 +55714,7 @@
         <v>97</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>185</v>
+        <v>308</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>25</v>
@@ -55939,7 +55967,7 @@
         <v>97</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>188</v>
+        <v>309</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>47</v>
@@ -55962,7 +55990,7 @@
         <v>97</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>190</v>
+        <v>310</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>49</v>
@@ -56017,7 +56045,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A26" s="16">
         <v>25</v>
       </c>
@@ -56030,8 +56058,8 @@
       <c r="D26" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="E26" s="16" t="s">
-        <v>184</v>
+      <c r="E26" s="20" t="s">
+        <v>311</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>55</v>
@@ -56474,8 +56502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9A5590-6272-4B80-B830-B6A31702A66E}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -56484,7 +56512,7 @@
     <col min="2" max="2" width="14.44140625" style="15"/>
     <col min="3" max="3" width="12.77734375" style="15" customWidth="1"/>
     <col min="4" max="4" width="4.109375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="255.77734375" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.33203125" style="15" customWidth="1"/>
     <col min="7" max="16384" width="14.44140625" style="15"/>
   </cols>
@@ -57135,7 +57163,7 @@
         <v>97</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="F31" s="16" t="s">
         <v>65</v>
@@ -57443,7 +57471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6300F22-321F-437F-A665-DB70574A8E8F}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -57453,7 +57481,7 @@
     <col min="2" max="2" width="14.44140625" style="15"/>
     <col min="3" max="3" width="11.21875" style="15" customWidth="1"/>
     <col min="4" max="4" width="4.21875" style="15" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="42.21875" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.33203125" style="15" customWidth="1"/>
     <col min="7" max="16384" width="14.44140625" style="15"/>
   </cols>
@@ -58410,8 +58438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{019FA4BB-587E-4B2A-B9AB-CF6EF1CB9C1A}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -58420,7 +58448,7 @@
     <col min="2" max="2" width="14.44140625" style="15"/>
     <col min="3" max="3" width="12.33203125" style="15" customWidth="1"/>
     <col min="4" max="4" width="4.77734375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="255.77734375" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.33203125" style="15" customWidth="1"/>
     <col min="7" max="16384" width="14.44140625" style="15"/>
   </cols>
@@ -58882,7 +58910,7 @@
         <v>97</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>47</v>
@@ -58905,7 +58933,7 @@
         <v>97</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>49</v>

</xml_diff>